<commit_message>
Done day 8, 9, and 10
</commit_message>
<xml_diff>
--- a/Day08/Lab08MT.xlsx
+++ b/Day08/Lab08MT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\gitRepo\DATA101\Day08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E4F2130-58EA-4FBF-9179-1B0381111DA2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{84FDDE85-7BA7-463D-9A67-42293F642160}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" tabRatio="938" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" tabRatio="938" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specs" sheetId="4" r:id="rId1"/>
@@ -314,9 +314,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -815,14 +815,14 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="333">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -1445,11 +1445,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2220000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1574,7 +1574,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3695,7 +3695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1130CF6-9D4F-475D-B5F1-D6E81BBDBBDC}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -4514,8 +4514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C5078F-7313-4A43-BC2F-5168E882596B}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>